<commit_message>
Re-do scenario buttons to match profile buttons
</commit_message>
<xml_diff>
--- a/data/ResearchProjectSpreadsheet_ReadForm.xlsx
+++ b/data/ResearchProjectSpreadsheet_ReadForm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daxledesma/Documents/GitHub/tdot-gi-streamlit/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97DA5D1-9F01-3742-9E32-E89E5E1C4A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07B185CB-5842-BF4C-8CED-2AD2A2E0C7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8960" yWindow="3480" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{B220E2DF-F534-4A75-BFA7-DDC35956FE64}"/>
+    <workbookView xWindow="0" yWindow="-21600" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{B220E2DF-F534-4A75-BFA7-DDC35956FE64}"/>
   </bookViews>
   <sheets>
     <sheet name="GI" sheetId="5" r:id="rId1"/>
@@ -993,9 +993,6 @@
     <t>Flooding reduction</t>
   </si>
   <si>
-    <t>Total Suspended Solids (TSS)</t>
-  </si>
-  <si>
     <t>Installation Cost Range</t>
   </si>
   <si>
@@ -1005,15 +1002,6 @@
     <t>Open Graded Friction Course</t>
   </si>
   <si>
-    <t>Metals</t>
-  </si>
-  <si>
-    <t>Total Phosphorous (TP)</t>
-  </si>
-  <si>
-    <t>Total Nitrogen (TN)</t>
-  </si>
-  <si>
     <t>Cost Considerations</t>
   </si>
   <si>
@@ -1098,9 +1086,6 @@
     <t>Contributing Drainage Area</t>
   </si>
   <si>
-    <t>max. (acre) or ratio</t>
-  </si>
-  <si>
     <t>https://www.sciencedirect.com/science/article/pii/S2046043018301333</t>
   </si>
   <si>
@@ -1200,9 +1185,6 @@
     <t>&lt;1</t>
   </si>
   <si>
-    <t>%  impervious area space reqd</t>
-  </si>
-  <si>
     <t>Range 10-20%</t>
   </si>
   <si>
@@ -1254,9 +1236,6 @@
     <t>Range 93%-100%</t>
   </si>
   <si>
-    <t>Organism removal</t>
-  </si>
-  <si>
     <t>Range 94%-100%</t>
   </si>
   <si>
@@ -1278,9 +1257,6 @@
     <t xml:space="preserve">C, D except w/ underdrain </t>
   </si>
   <si>
-    <t>10 max</t>
-  </si>
-  <si>
     <t>5:1</t>
   </si>
   <si>
@@ -1446,9 +1422,6 @@
     <t>50% than turf</t>
   </si>
   <si>
-    <t>Indefinately</t>
-  </si>
-  <si>
     <t>per acre per yr</t>
   </si>
   <si>
@@ -1624,6 +1597,33 @@
   </si>
   <si>
     <t>100 - 1200</t>
+  </si>
+  <si>
+    <t>Maximum (acre) or ratio</t>
+  </si>
+  <si>
+    <t>Minimum %  impervious area space reqd</t>
+  </si>
+  <si>
+    <t>0-10</t>
+  </si>
+  <si>
+    <t>Total Suspended Solids (TSS) (Minimum required)</t>
+  </si>
+  <si>
+    <t>Total Phosphorous (TP) (Minimum required)</t>
+  </si>
+  <si>
+    <t>Total Nitrogen (TN) (Minimum required)</t>
+  </si>
+  <si>
+    <t>Metals (Minimum required)</t>
+  </si>
+  <si>
+    <t>Organism removal (Minimum required)</t>
+  </si>
+  <si>
+    <t>Indefinitely</t>
   </si>
 </sst>
 </file>
@@ -9158,13 +9158,13 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C36" s="102" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -9172,13 +9172,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="C37" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -9186,13 +9186,13 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="C38" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -9200,13 +9200,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="C39" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -9214,13 +9214,13 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="C40" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="D40" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -9228,13 +9228,13 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
       <c r="C41" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -9242,24 +9242,24 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>490</v>
+        <v>481</v>
       </c>
       <c r="C42" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>489</v>
+        <v>480</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="B43" t="s">
-        <v>495</v>
+        <v>486</v>
       </c>
       <c r="C43" t="s">
-        <v>496</v>
+        <v>487</v>
       </c>
       <c r="D43" t="s">
-        <v>494</v>
+        <v>485</v>
       </c>
     </row>
   </sheetData>
@@ -10716,9 +10716,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68FC19DD-5760-497F-BD45-2976AF50B657}">
   <dimension ref="A1:AU62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="118" zoomScaleNormal="75" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="75" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="W1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AE30" sqref="AE30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -10760,7 +10760,7 @@
     <row r="1" spans="1:47" s="105" customFormat="1" ht="14.5" customHeight="1">
       <c r="A1" s="106"/>
       <c r="B1" s="155" t="s">
-        <v>500</v>
+        <v>491</v>
       </c>
       <c r="C1" s="106"/>
       <c r="D1" s="122"/>
@@ -10798,34 +10798,34 @@
     <row r="2" spans="1:47" ht="17.5" customHeight="1">
       <c r="A2" s="122"/>
       <c r="B2" s="221" t="s">
-        <v>500</v>
+        <v>491</v>
       </c>
       <c r="C2" s="212" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="D2" s="213"/>
       <c r="E2" s="213"/>
       <c r="F2" s="214"/>
       <c r="G2" s="212" t="s">
-        <v>480</v>
+        <v>471</v>
       </c>
       <c r="H2" s="213"/>
       <c r="I2" s="213"/>
       <c r="J2" s="213"/>
       <c r="K2" s="213"/>
       <c r="L2" s="213" t="s">
-        <v>481</v>
+        <v>472</v>
       </c>
       <c r="M2" s="214"/>
       <c r="N2" s="212" t="s">
-        <v>482</v>
+        <v>473</v>
       </c>
       <c r="O2" s="213"/>
       <c r="P2" s="213"/>
       <c r="Q2" s="213"/>
       <c r="R2" s="214"/>
       <c r="S2" s="211" t="s">
-        <v>478</v>
+        <v>469</v>
       </c>
       <c r="T2" s="211"/>
       <c r="U2" s="211"/>
@@ -10833,7 +10833,7 @@
       <c r="W2" s="211"/>
       <c r="X2" s="211"/>
       <c r="Y2" s="211" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="Z2" s="211"/>
       <c r="AA2" s="211"/>
@@ -10841,7 +10841,7 @@
       <c r="AC2" s="211"/>
       <c r="AD2" s="211"/>
       <c r="AE2" s="128" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="AF2" s="212" t="s">
         <v>116</v>
@@ -10855,125 +10855,125 @@
       </c>
       <c r="B3" s="222"/>
       <c r="C3" s="148" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="D3" s="148" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="E3" s="217" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="F3" s="219"/>
       <c r="G3" s="148" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="H3" s="148" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="I3" s="217" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="J3" s="219"/>
       <c r="K3" s="148" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="L3" s="148" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="M3" s="148" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="N3" s="215" t="s">
-        <v>300</v>
+        <v>505</v>
       </c>
       <c r="O3" s="215" t="s">
-        <v>305</v>
+        <v>506</v>
       </c>
       <c r="P3" s="215" t="s">
-        <v>306</v>
+        <v>507</v>
       </c>
       <c r="Q3" s="215" t="s">
-        <v>304</v>
+        <v>508</v>
       </c>
       <c r="R3" s="215" t="s">
-        <v>387</v>
+        <v>509</v>
       </c>
       <c r="S3" s="220" t="s">
         <v>299</v>
       </c>
       <c r="T3" s="220" t="s">
-        <v>471</v>
+        <v>462</v>
       </c>
       <c r="U3" s="220" t="s">
-        <v>472</v>
+        <v>463</v>
       </c>
       <c r="V3" s="220" t="s">
-        <v>473</v>
+        <v>464</v>
       </c>
       <c r="W3" s="220" t="s">
-        <v>474</v>
+        <v>465</v>
       </c>
       <c r="X3" s="220" t="s">
-        <v>475</v>
+        <v>466</v>
       </c>
       <c r="Y3" s="217" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="Z3" s="218"/>
       <c r="AA3" s="219"/>
       <c r="AB3" s="217" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="AC3" s="218"/>
       <c r="AD3" s="218"/>
       <c r="AE3" s="147" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="AF3" s="223" t="s">
-        <v>486</v>
+        <v>477</v>
       </c>
       <c r="AG3" s="215" t="s">
-        <v>487</v>
+        <v>478</v>
       </c>
       <c r="AH3" s="215" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="4" spans="1:47" ht="17" thickBot="1">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="4" spans="1:47" ht="33" thickBot="1">
       <c r="A4" s="108"/>
       <c r="B4" s="156"/>
       <c r="C4" s="150" t="s">
+        <v>315</v>
+      </c>
+      <c r="D4" s="150" t="s">
+        <v>315</v>
+      </c>
+      <c r="E4" s="149" t="s">
+        <v>502</v>
+      </c>
+      <c r="F4" s="149" t="s">
+        <v>503</v>
+      </c>
+      <c r="G4" s="150" t="s">
         <v>319</v>
       </c>
-      <c r="D4" s="150" t="s">
+      <c r="H4" s="150" t="s">
         <v>319</v>
       </c>
-      <c r="E4" s="149" t="s">
-        <v>335</v>
-      </c>
-      <c r="F4" s="149" t="s">
-        <v>369</v>
-      </c>
-      <c r="G4" s="150" t="s">
-        <v>323</v>
-      </c>
-      <c r="H4" s="150" t="s">
-        <v>323</v>
-      </c>
       <c r="I4" s="150" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="J4" s="150" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="K4" s="150" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="L4" s="150" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="M4" s="150" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="N4" s="216"/>
       <c r="O4" s="216"/>
@@ -10987,25 +10987,25 @@
       <c r="W4" s="216"/>
       <c r="X4" s="216"/>
       <c r="Y4" s="151" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="Z4" s="152" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="AA4" s="152" t="s">
         <v>10</v>
       </c>
       <c r="AB4" s="153" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="AC4" s="153" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="AD4" s="153" t="s">
         <v>10</v>
       </c>
       <c r="AE4" s="146" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="AF4" s="224"/>
       <c r="AG4" s="216"/>
@@ -11013,7 +11013,7 @@
     </row>
     <row r="5" spans="1:47" s="107" customFormat="1" ht="15.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A5" s="198" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="B5" s="157" t="s">
         <v>38</v>
@@ -11022,7 +11022,7 @@
         <v>0.05</v>
       </c>
       <c r="D5" s="117" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="E5" s="111">
         <v>5</v>
@@ -11033,16 +11033,16 @@
       </c>
       <c r="H5" s="111"/>
       <c r="I5" s="111" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="J5" s="111" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="K5" s="111">
         <v>2</v>
       </c>
       <c r="L5" s="209" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
       <c r="M5" s="111">
         <v>50</v>
@@ -11051,44 +11051,44 @@
         <v>0.37</v>
       </c>
       <c r="O5" s="130" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="P5" s="130">
         <v>0.14000000000000001</v>
       </c>
       <c r="Q5" s="130"/>
       <c r="R5" s="130" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="S5" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="T5" s="111" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="U5" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="V5" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="W5" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="X5" s="109" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
       <c r="Y5" s="114"/>
       <c r="Z5" s="115"/>
       <c r="AA5" s="116"/>
       <c r="AB5" s="115" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="AC5" s="115" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="AD5" s="116" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="AE5" s="111"/>
       <c r="AF5" s="131"/>
@@ -11117,30 +11117,30 @@
         <v>0.05</v>
       </c>
       <c r="D6" s="117" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="E6" s="122" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="F6" s="111" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="G6" s="111">
         <v>0.5</v>
       </c>
       <c r="H6" s="111"/>
       <c r="I6" s="111" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="J6" s="111" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="K6" s="111">
         <v>2</v>
       </c>
       <c r="L6" s="210"/>
       <c r="M6" s="111" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="N6" s="109">
         <v>0.85</v>
@@ -11158,40 +11158,40 @@
         <v>0.6</v>
       </c>
       <c r="S6" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="T6" s="111" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="U6" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="V6" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="W6" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="X6" s="109">
         <v>0.5</v>
       </c>
       <c r="Y6" s="114" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="Z6" s="115" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="AA6" s="116" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="AB6" s="115" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="AC6" s="115" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="AD6" s="116" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="AE6" s="111"/>
       <c r="AF6" s="111"/>
@@ -11214,13 +11214,13 @@
     <row r="7" spans="1:47" s="105" customFormat="1" ht="15" customHeight="1" thickBot="1">
       <c r="A7" s="201"/>
       <c r="B7" s="159" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="C7" s="109">
         <v>0.08</v>
       </c>
       <c r="D7" s="110" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="E7" s="111">
         <v>2</v>
@@ -11229,19 +11229,19 @@
         <v>0.04</v>
       </c>
       <c r="G7" s="112" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
       <c r="H7" s="111">
         <v>10</v>
       </c>
       <c r="I7" s="111" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="J7" s="111" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="K7" s="111" t="s">
-        <v>395</v>
+        <v>504</v>
       </c>
       <c r="L7" s="111">
         <v>10</v>
@@ -11259,26 +11259,26 @@
         <v>0.4</v>
       </c>
       <c r="Q7" s="111" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
       <c r="R7" s="111"/>
       <c r="S7" s="111" t="s">
-        <v>483</v>
+        <v>474</v>
       </c>
       <c r="T7" s="111" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
       <c r="U7" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="V7" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="W7" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="X7" s="111" t="s">
-        <v>497</v>
+        <v>488</v>
       </c>
       <c r="Y7" s="114">
         <v>1.5</v>
@@ -11287,19 +11287,19 @@
         <v>6</v>
       </c>
       <c r="AA7" s="116" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="AB7" s="115" t="s">
-        <v>499</v>
+        <v>490</v>
       </c>
       <c r="AC7" s="115" t="s">
-        <v>499</v>
+        <v>490</v>
       </c>
       <c r="AD7" s="116" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="AE7" s="111" t="s">
-        <v>498</v>
+        <v>489</v>
       </c>
       <c r="AF7" s="111"/>
       <c r="AG7" s="111"/>
@@ -11308,29 +11308,29 @@
     <row r="8" spans="1:47" s="105" customFormat="1" ht="15" customHeight="1" thickBot="1">
       <c r="A8" s="201"/>
       <c r="B8" s="160" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="C8" s="109">
         <v>0.2</v>
       </c>
       <c r="D8" s="117" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="E8" s="111">
         <v>5</v>
       </c>
       <c r="F8" s="109" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="G8" s="111">
         <v>0.5</v>
       </c>
       <c r="H8" s="111"/>
       <c r="I8" s="111" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="J8" s="111" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="K8" s="111">
         <v>2</v>
@@ -11339,52 +11339,52 @@
         <v>10</v>
       </c>
       <c r="M8" s="111" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="N8" s="109" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
       <c r="O8" s="109" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="P8" s="109" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="Q8" s="109" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="R8" s="109" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
       <c r="S8" s="111"/>
       <c r="T8" s="111" t="s">
-        <v>484</v>
+        <v>475</v>
       </c>
       <c r="U8" s="111"/>
       <c r="V8" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="W8" s="111"/>
       <c r="X8" s="109" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
       <c r="Y8" s="114" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="Z8" s="114" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="AA8" s="111" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="AB8" s="111" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="AC8" s="111" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="AD8" s="116" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="AE8" s="111"/>
       <c r="AF8" s="111"/>
@@ -11400,7 +11400,7 @@
         <v>0.04</v>
       </c>
       <c r="D9" s="110" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="E9" s="111">
         <v>2</v>
@@ -11415,13 +11415,13 @@
         <v>10</v>
       </c>
       <c r="I9" s="111" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="J9" s="111" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="K9" s="111" t="s">
-        <v>395</v>
+        <v>504</v>
       </c>
       <c r="L9" s="111">
         <v>10</v>
@@ -11439,7 +11439,7 @@
       <c r="U9" s="111"/>
       <c r="V9" s="111"/>
       <c r="W9" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="X9" s="111"/>
       <c r="Y9" s="114">
@@ -11449,7 +11449,7 @@
         <v>16</v>
       </c>
       <c r="AA9" s="116" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="AB9" s="115">
         <v>0.31</v>
@@ -11458,10 +11458,10 @@
         <v>0.61</v>
       </c>
       <c r="AD9" s="116" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="AE9" s="111" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="AF9" s="111"/>
       <c r="AG9" s="111"/>
@@ -11469,32 +11469,32 @@
     </row>
     <row r="10" spans="1:47" s="107" customFormat="1" ht="15" customHeight="1" thickBot="1">
       <c r="A10" s="198" t="s">
-        <v>463</v>
+        <v>454</v>
       </c>
       <c r="B10" s="158" t="s">
-        <v>461</v>
+        <v>452</v>
       </c>
       <c r="C10" s="109">
         <v>0.04</v>
       </c>
       <c r="D10" s="117" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="E10" s="111">
         <v>5</v>
       </c>
       <c r="F10" s="109" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="G10" s="111">
         <v>0.5</v>
       </c>
       <c r="H10" s="111"/>
       <c r="I10" s="111" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="J10" s="111" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="K10" s="111">
         <v>2</v>
@@ -11503,54 +11503,54 @@
         <v>10</v>
       </c>
       <c r="M10" s="111" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="N10" s="113" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
       <c r="O10" s="113" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
       <c r="P10" s="113" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
       <c r="Q10" s="113" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
       <c r="R10" s="109" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="S10" s="111" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="T10" s="111" t="s">
-        <v>484</v>
+        <v>475</v>
       </c>
       <c r="U10" s="111"/>
       <c r="V10" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="W10" s="111"/>
       <c r="X10" s="113" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
       <c r="Y10" s="114" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="Z10" s="114" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="AA10" s="116" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="AB10" s="115" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="AC10" s="115" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="AD10" s="116" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="AE10" s="111"/>
       <c r="AF10" s="111"/>
@@ -11573,38 +11573,38 @@
     <row r="11" spans="1:47" s="107" customFormat="1" ht="15" customHeight="1" thickBot="1">
       <c r="A11" s="199"/>
       <c r="B11" s="158" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
       <c r="C11" s="109">
         <v>0.04</v>
       </c>
       <c r="D11" s="117" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="E11" s="111">
         <v>5</v>
       </c>
       <c r="F11" s="109" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="G11" s="111">
         <v>0.5</v>
       </c>
       <c r="H11" s="111"/>
       <c r="I11" s="111" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="J11" s="111" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="K11" s="111" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="L11" s="111">
         <v>10</v>
       </c>
       <c r="M11" s="111" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="N11" s="113">
         <v>0.8</v>
@@ -11619,17 +11619,17 @@
         <v>0.2</v>
       </c>
       <c r="R11" s="109" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="S11" s="111" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="T11" s="111" t="s">
-        <v>484</v>
+        <v>475</v>
       </c>
       <c r="U11" s="111"/>
       <c r="V11" s="111" t="s">
-        <v>483</v>
+        <v>474</v>
       </c>
       <c r="W11" s="111"/>
       <c r="X11" s="109">
@@ -11642,16 +11642,16 @@
         <v>30000</v>
       </c>
       <c r="AA11" s="116" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="AB11" s="115" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="AC11" s="115" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="AD11" s="116" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="AE11" s="111"/>
       <c r="AF11" s="111"/>
@@ -11673,7 +11673,7 @@
     </row>
     <row r="12" spans="1:47" s="107" customFormat="1" ht="15" customHeight="1" thickBot="1">
       <c r="A12" s="119" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="B12" s="157"/>
       <c r="C12" s="109">
@@ -11683,7 +11683,7 @@
         <v>0.02</v>
       </c>
       <c r="E12" s="110" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="F12" s="109">
         <v>0.2</v>
@@ -11693,49 +11693,49 @@
       </c>
       <c r="H12" s="111"/>
       <c r="I12" s="111" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="J12" s="111" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="K12" s="111" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="L12" s="111">
         <v>10</v>
       </c>
       <c r="M12" s="111" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="N12" s="113" t="s">
-        <v>464</v>
+        <v>455</v>
       </c>
       <c r="O12" s="109">
         <v>0.2</v>
       </c>
       <c r="P12" s="109" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="Q12" s="109">
         <v>0.4</v>
       </c>
       <c r="R12" s="109" t="s">
+        <v>308</v>
+      </c>
+      <c r="S12" s="111" t="s">
+        <v>313</v>
+      </c>
+      <c r="T12" s="111" t="s">
+        <v>313</v>
+      </c>
+      <c r="U12" s="111" t="s">
+        <v>313</v>
+      </c>
+      <c r="V12" s="111" t="s">
         <v>312</v>
       </c>
-      <c r="S12" s="111" t="s">
-        <v>317</v>
-      </c>
-      <c r="T12" s="111" t="s">
-        <v>317</v>
-      </c>
-      <c r="U12" s="111" t="s">
-        <v>317</v>
-      </c>
-      <c r="V12" s="111" t="s">
-        <v>316</v>
-      </c>
       <c r="W12" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="X12" s="109">
         <v>0.25</v>
@@ -11747,7 +11747,7 @@
         <v>3.33</v>
       </c>
       <c r="AA12" s="111" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="AB12" s="114">
         <v>0.01</v>
@@ -11756,10 +11756,10 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AD12" s="116" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="AE12" s="111" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="AF12" s="111"/>
       <c r="AG12" s="111"/>
@@ -11780,16 +11780,16 @@
     </row>
     <row r="13" spans="1:47" s="107" customFormat="1" ht="15" customHeight="1" thickBot="1">
       <c r="A13" s="202" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="B13" s="162" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="C13" s="109">
         <v>0.04</v>
       </c>
       <c r="D13" s="117" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="E13" s="111">
         <v>5</v>
@@ -11802,10 +11802,10 @@
       </c>
       <c r="H13" s="111"/>
       <c r="I13" s="111" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="J13" s="111" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="K13" s="111">
         <v>2</v>
@@ -11814,7 +11814,7 @@
         <v>10</v>
       </c>
       <c r="M13" s="111" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="N13" s="113">
         <v>0.5</v>
@@ -11829,43 +11829,43 @@
         <v>0.3</v>
       </c>
       <c r="R13" s="109" t="s">
+        <v>308</v>
+      </c>
+      <c r="S13" s="111" t="s">
+        <v>313</v>
+      </c>
+      <c r="T13" s="111" t="s">
+        <v>313</v>
+      </c>
+      <c r="U13" s="111" t="s">
         <v>312</v>
       </c>
-      <c r="S13" s="111" t="s">
-        <v>317</v>
-      </c>
-      <c r="T13" s="111" t="s">
-        <v>317</v>
-      </c>
-      <c r="U13" s="111" t="s">
-        <v>316</v>
-      </c>
       <c r="V13" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="W13" s="111" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="X13" s="109">
         <v>0.25</v>
       </c>
       <c r="Y13" s="114" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="Z13" s="114" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="AA13" s="111" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="AB13" s="114" t="s">
+        <v>356</v>
+      </c>
+      <c r="AC13" s="114" t="s">
+        <v>308</v>
+      </c>
+      <c r="AD13" s="116" t="s">
         <v>361</v>
-      </c>
-      <c r="AC13" s="114" t="s">
-        <v>312</v>
-      </c>
-      <c r="AD13" s="116" t="s">
-        <v>366</v>
       </c>
       <c r="AE13" s="111"/>
       <c r="AF13" s="111"/>
@@ -11888,13 +11888,13 @@
     <row r="14" spans="1:47" s="107" customFormat="1" ht="15" customHeight="1" thickBot="1">
       <c r="A14" s="203"/>
       <c r="B14" s="162" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="C14" s="109">
         <v>0.04</v>
       </c>
       <c r="D14" s="117" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="E14" s="111">
         <v>5</v>
@@ -11907,10 +11907,10 @@
       </c>
       <c r="H14" s="111"/>
       <c r="I14" s="111" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="J14" s="111" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="K14" s="111">
         <v>2</v>
@@ -11919,7 +11919,7 @@
         <v>10</v>
       </c>
       <c r="M14" s="111" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="N14" s="113">
         <v>0.5</v>
@@ -11934,41 +11934,41 @@
         <v>0.3</v>
       </c>
       <c r="R14" s="109" t="s">
+        <v>308</v>
+      </c>
+      <c r="S14" s="111" t="s">
+        <v>313</v>
+      </c>
+      <c r="T14" s="111" t="s">
+        <v>313</v>
+      </c>
+      <c r="U14" s="111" t="s">
         <v>312</v>
       </c>
-      <c r="S14" s="111" t="s">
-        <v>317</v>
-      </c>
-      <c r="T14" s="111" t="s">
-        <v>317</v>
-      </c>
-      <c r="U14" s="111" t="s">
-        <v>316</v>
-      </c>
       <c r="V14" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="W14" s="111"/>
       <c r="X14" s="109">
         <v>0.1</v>
       </c>
       <c r="Y14" s="114" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="Z14" s="114" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="AA14" s="111" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="AB14" s="114" t="s">
+        <v>356</v>
+      </c>
+      <c r="AC14" s="114" t="s">
+        <v>308</v>
+      </c>
+      <c r="AD14" s="116" t="s">
         <v>361</v>
-      </c>
-      <c r="AC14" s="114" t="s">
-        <v>312</v>
-      </c>
-      <c r="AD14" s="116" t="s">
-        <v>366</v>
       </c>
       <c r="AE14" s="111"/>
       <c r="AF14" s="111"/>
@@ -11990,10 +11990,10 @@
     </row>
     <row r="15" spans="1:47" ht="14.5" customHeight="1">
       <c r="A15" s="204" t="s">
-        <v>479</v>
+        <v>470</v>
       </c>
       <c r="B15" s="161" t="s">
-        <v>509</v>
+        <v>500</v>
       </c>
       <c r="C15" s="109">
         <v>0.06</v>
@@ -12005,7 +12005,7 @@
         <v>15</v>
       </c>
       <c r="F15" s="133" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="G15" s="111">
         <v>0.5</v>
@@ -12014,13 +12014,13 @@
         <v>6.4</v>
       </c>
       <c r="I15" s="111" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="J15" s="111" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="K15" s="111" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="L15" s="111">
         <v>10</v>
@@ -12029,37 +12029,37 @@
         <v>100</v>
       </c>
       <c r="N15" s="113" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="O15" s="113" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="P15" s="109" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="Q15" s="109" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="R15" s="109" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="S15" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="T15" s="111" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="U15" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="V15" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="W15" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="X15" s="109" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="Y15" s="114">
         <v>5.5</v>
@@ -12068,7 +12068,7 @@
         <v>28</v>
       </c>
       <c r="AA15" s="111" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="AB15" s="114">
         <v>0.09</v>
@@ -12077,10 +12077,10 @@
         <v>0.23</v>
       </c>
       <c r="AD15" s="116" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="AE15" s="111" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="AF15" s="111"/>
       <c r="AG15" s="111"/>
@@ -12089,7 +12089,7 @@
     <row r="16" spans="1:47" s="104" customFormat="1" ht="14.5" customHeight="1">
       <c r="A16" s="205"/>
       <c r="B16" s="163" t="s">
-        <v>508</v>
+        <v>499</v>
       </c>
       <c r="C16" s="109">
         <v>0.06</v>
@@ -12101,7 +12101,7 @@
         <v>15</v>
       </c>
       <c r="F16" s="133" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="G16" s="111">
         <v>0.5</v>
@@ -12110,13 +12110,13 @@
         <v>6.4</v>
       </c>
       <c r="I16" s="111" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="J16" s="111" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="K16" s="111" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="L16" s="111">
         <v>10</v>
@@ -12125,37 +12125,37 @@
         <v>100</v>
       </c>
       <c r="N16" s="113" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="O16" s="113" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="P16" s="109" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="Q16" s="109" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="R16" s="109" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="S16" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="T16" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="U16" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="V16" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="W16" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="X16" s="109" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="Y16" s="114">
         <v>5.5</v>
@@ -12164,7 +12164,7 @@
         <v>28</v>
       </c>
       <c r="AA16" s="111" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="AB16" s="114">
         <v>0.09</v>
@@ -12173,10 +12173,10 @@
         <v>0.23</v>
       </c>
       <c r="AD16" s="116" t="s">
+        <v>344</v>
+      </c>
+      <c r="AE16" s="111" t="s">
         <v>349</v>
-      </c>
-      <c r="AE16" s="111" t="s">
-        <v>354</v>
       </c>
       <c r="AF16" s="111"/>
       <c r="AG16" s="111"/>
@@ -12198,7 +12198,7 @@
     <row r="17" spans="1:47" ht="14.5" customHeight="1">
       <c r="A17" s="205"/>
       <c r="B17" s="163" t="s">
-        <v>507</v>
+        <v>498</v>
       </c>
       <c r="C17" s="109">
         <v>0.06</v>
@@ -12210,7 +12210,7 @@
         <v>15</v>
       </c>
       <c r="F17" s="133" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="G17" s="111">
         <v>0.5</v>
@@ -12219,13 +12219,13 @@
         <v>6.4</v>
       </c>
       <c r="I17" s="111" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="J17" s="111" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="K17" s="111" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="L17" s="111">
         <v>10</v>
@@ -12237,34 +12237,34 @@
         <v>0.8</v>
       </c>
       <c r="O17" s="113" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="P17" s="109" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="Q17" s="109" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="R17" s="109" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="S17" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="T17" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="U17" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="V17" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="W17" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="X17" s="109" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="Y17" s="114">
         <v>5.3</v>
@@ -12273,7 +12273,7 @@
         <v>34</v>
       </c>
       <c r="AA17" s="111" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="AB17" s="114">
         <v>0.01</v>
@@ -12282,10 +12282,10 @@
         <v>0.23</v>
       </c>
       <c r="AD17" s="116" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="AE17" s="111" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="AF17" s="111"/>
       <c r="AG17" s="111"/>
@@ -12294,7 +12294,7 @@
     <row r="18" spans="1:47" ht="14.5" customHeight="1">
       <c r="A18" s="205"/>
       <c r="B18" s="164" t="s">
-        <v>506</v>
+        <v>497</v>
       </c>
       <c r="C18" s="109">
         <v>0.06</v>
@@ -12306,7 +12306,7 @@
         <v>15</v>
       </c>
       <c r="F18" s="133" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="G18" s="111">
         <v>0.5</v>
@@ -12315,13 +12315,13 @@
         <v>6.4</v>
       </c>
       <c r="I18" s="111" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="J18" s="111" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="K18" s="111" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="L18" s="111">
         <v>10</v>
@@ -12333,34 +12333,34 @@
         <v>0.8</v>
       </c>
       <c r="O18" s="113" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="P18" s="109" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="Q18" s="109" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="R18" s="109" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="S18" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="T18" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="U18" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="V18" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="W18" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="X18" s="109" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="Y18" s="114">
         <v>5.3</v>
@@ -12369,7 +12369,7 @@
         <v>12</v>
       </c>
       <c r="AA18" s="111" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="AB18" s="114">
         <v>0.01</v>
@@ -12378,10 +12378,10 @@
         <v>0.23</v>
       </c>
       <c r="AD18" s="116" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="AE18" s="111" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="AF18" s="111"/>
       <c r="AG18" s="111"/>
@@ -12390,7 +12390,7 @@
     <row r="19" spans="1:47" ht="15" customHeight="1" thickBot="1">
       <c r="A19" s="206"/>
       <c r="B19" s="159" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C19" s="109">
         <v>0.05</v>
@@ -12399,7 +12399,7 @@
         <v>0.02</v>
       </c>
       <c r="E19" s="111" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="F19" s="109">
         <v>0</v>
@@ -12411,13 +12411,13 @@
         <v>6.4</v>
       </c>
       <c r="I19" s="111" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="J19" s="111" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="K19" s="111" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="L19" s="111">
         <v>10</v>
@@ -12429,50 +12429,50 @@
         <v>0.5</v>
       </c>
       <c r="O19" s="109" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="P19" s="109" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="Q19" s="109" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="R19" s="109" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="S19" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="T19" s="111" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="U19" s="111"/>
       <c r="V19" s="111" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="W19" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="X19" s="109">
         <v>0</v>
       </c>
       <c r="Y19" s="114" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="Z19" s="114" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="AA19" s="111" t="s">
+        <v>308</v>
+      </c>
+      <c r="AB19" s="114" t="s">
         <v>312</v>
       </c>
-      <c r="AB19" s="114" t="s">
-        <v>316</v>
-      </c>
       <c r="AC19" s="114" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="AD19" s="116" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="AE19" s="111"/>
       <c r="AF19" s="111"/>
@@ -12481,43 +12481,43 @@
     </row>
     <row r="20" spans="1:47" s="105" customFormat="1" ht="14.5" customHeight="1">
       <c r="A20" s="198" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="B20" s="161" t="s">
-        <v>505</v>
+        <v>496</v>
       </c>
       <c r="C20" s="109">
         <v>0.15</v>
       </c>
       <c r="D20" s="117" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="E20" s="111" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="F20" s="117" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="G20" s="111" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="H20" s="111" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
       <c r="I20" s="111" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
       <c r="J20" s="111" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
       <c r="K20" s="111">
         <v>2</v>
       </c>
       <c r="L20" s="207" t="s">
-        <v>460</v>
+        <v>451</v>
       </c>
       <c r="M20" s="111" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="N20" s="109">
         <v>0.65</v>
@@ -12529,28 +12529,28 @@
         <v>0.2</v>
       </c>
       <c r="Q20" s="109" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
       <c r="R20" s="109" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
       <c r="S20" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="T20" s="111" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="U20" s="111" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
       <c r="V20" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="W20" s="111" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="X20" s="109" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
       <c r="Y20" s="114">
         <v>42000</v>
@@ -12559,7 +12559,7 @@
         <v>1400000</v>
       </c>
       <c r="AA20" s="111" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="AB20" s="109">
         <v>0.03</v>
@@ -12568,10 +12568,10 @@
         <v>0.05</v>
       </c>
       <c r="AD20" s="116" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="AE20" s="111" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="AF20" s="111"/>
       <c r="AG20" s="111"/>
@@ -12580,41 +12580,41 @@
     <row r="21" spans="1:47" s="105" customFormat="1" ht="15" customHeight="1" thickBot="1">
       <c r="A21" s="201"/>
       <c r="B21" s="159" t="s">
-        <v>504</v>
+        <v>495</v>
       </c>
       <c r="C21" s="109">
         <v>0.15</v>
       </c>
       <c r="D21" s="117" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="E21" s="111" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
       <c r="F21" s="109" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="G21" s="111" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="H21" s="111" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
       <c r="I21" s="111" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
       <c r="J21" s="111" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="K21" s="111">
         <v>2</v>
       </c>
       <c r="L21" s="208"/>
       <c r="M21" s="111" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="N21" s="109" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
       <c r="O21" s="109">
         <v>0.6</v>
@@ -12623,37 +12623,37 @@
         <v>0.3</v>
       </c>
       <c r="Q21" s="109" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
       <c r="R21" s="109" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
       <c r="S21" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="T21" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="U21" s="111" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
       <c r="V21" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="W21" s="111" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="X21" s="109" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
       <c r="Y21" s="114" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
       <c r="Z21" s="114">
         <v>50000</v>
       </c>
       <c r="AA21" s="111" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="AB21" s="109">
         <v>0.03</v>
@@ -12662,10 +12662,10 @@
         <v>0.05</v>
       </c>
       <c r="AD21" s="116" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="AE21" s="111" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
       <c r="AF21" s="111"/>
       <c r="AG21" s="111"/>
@@ -12674,13 +12674,13 @@
     <row r="22" spans="1:47" s="107" customFormat="1" ht="15" customHeight="1" thickBot="1">
       <c r="A22" s="199"/>
       <c r="B22" s="162" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="C22" s="109">
         <v>0.15</v>
       </c>
       <c r="D22" s="117" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="E22" s="111">
         <v>10</v>
@@ -12689,10 +12689,10 @@
       <c r="G22" s="111"/>
       <c r="H22" s="111"/>
       <c r="I22" s="111" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="J22" s="111" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="K22" s="111">
         <v>2</v>
@@ -12715,20 +12715,20 @@
       <c r="Q22" s="109"/>
       <c r="R22" s="109"/>
       <c r="S22" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="T22" s="111"/>
       <c r="U22" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="V22" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="W22" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="X22" s="109" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="Y22" s="114">
         <v>25000</v>
@@ -12737,7 +12737,7 @@
         <v>50000</v>
       </c>
       <c r="AA22" s="111" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="AB22" s="109">
         <v>0.03</v>
@@ -12746,10 +12746,10 @@
         <v>0.05</v>
       </c>
       <c r="AD22" s="116" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="AE22" s="111" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="AF22" s="111"/>
       <c r="AG22" s="111"/>
@@ -12770,18 +12770,18 @@
     </row>
     <row r="23" spans="1:47" s="121" customFormat="1" ht="14.5" customHeight="1" thickBot="1">
       <c r="A23" s="144" t="s">
-        <v>476</v>
+        <v>467</v>
       </c>
       <c r="B23" s="162"/>
       <c r="C23" s="109">
         <v>0.01</v>
       </c>
       <c r="D23" s="109" t="s">
-        <v>477</v>
+        <v>468</v>
       </c>
       <c r="E23" s="111"/>
       <c r="F23" s="117" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="G23" s="111"/>
       <c r="H23" s="111"/>
@@ -12804,34 +12804,34 @@
       <c r="Q23" s="109"/>
       <c r="R23" s="109"/>
       <c r="S23" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="T23" s="111" t="s">
-        <v>484</v>
+        <v>475</v>
       </c>
       <c r="U23" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="V23" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="W23" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="X23" s="109" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="Y23" s="114" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="Z23" s="114" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="AA23" s="111" t="s">
+        <v>308</v>
+      </c>
+      <c r="AB23" s="111" t="s">
         <v>312</v>
-      </c>
-      <c r="AB23" s="111" t="s">
-        <v>316</v>
       </c>
       <c r="AC23" s="111"/>
       <c r="AD23" s="116"/>
@@ -12860,11 +12860,11 @@
       <c r="B24" s="162"/>
       <c r="C24" s="109"/>
       <c r="D24" s="110" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="E24" s="111"/>
       <c r="F24" s="109" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="G24" s="111"/>
       <c r="H24" s="111"/>
@@ -12874,39 +12874,39 @@
       <c r="L24" s="111"/>
       <c r="M24" s="111"/>
       <c r="N24" s="111" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="O24" s="111" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="P24" s="111" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="Q24" s="111"/>
       <c r="R24" s="111" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="S24" s="111"/>
       <c r="T24" s="111"/>
       <c r="U24" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="V24" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="W24" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="X24" s="109" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="Y24" s="114" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="Z24" s="114"/>
       <c r="AA24" s="111"/>
       <c r="AB24" s="114" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="AC24" s="114"/>
       <c r="AD24" s="116"/>
@@ -12937,32 +12937,32 @@
         <v>0.06</v>
       </c>
       <c r="D25" s="109" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="E25" s="111">
         <v>5</v>
       </c>
       <c r="F25" s="109" t="s">
-        <v>465</v>
+        <v>456</v>
       </c>
       <c r="G25" s="111">
         <v>0.5</v>
       </c>
       <c r="H25" s="111"/>
       <c r="I25" s="111" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="J25" s="111" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="K25" s="111">
         <v>4</v>
       </c>
       <c r="L25" s="111" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="M25" s="111" t="s">
-        <v>510</v>
+        <v>501</v>
       </c>
       <c r="N25" s="113">
         <v>0.85</v>
@@ -12980,40 +12980,40 @@
         <v>1</v>
       </c>
       <c r="S25" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="T25" s="111" t="s">
-        <v>484</v>
+        <v>475</v>
       </c>
       <c r="U25" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="V25" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="W25" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="X25" s="109" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="Y25" s="114" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="Z25" s="114" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="AA25" s="111" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="AB25" s="114" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="AC25" s="114" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="AD25" s="116" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="AE25" s="111"/>
       <c r="AF25" s="111"/>
@@ -13040,11 +13040,11 @@
       <c r="B26" s="162"/>
       <c r="C26" s="109"/>
       <c r="D26" s="110" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="E26" s="111"/>
       <c r="F26" s="109" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="G26" s="111"/>
       <c r="H26" s="111"/>
@@ -13093,71 +13093,71 @@
         <v>83</v>
       </c>
       <c r="B27" s="162" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="C27" s="109">
         <v>0.01</v>
       </c>
       <c r="D27" s="109" t="s">
-        <v>488</v>
+        <v>479</v>
       </c>
       <c r="E27" s="111" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="F27" s="109" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="G27" s="111" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="H27" s="111" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
       <c r="I27" s="111" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
       <c r="J27" s="111" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
       <c r="K27" s="111">
         <v>2</v>
       </c>
       <c r="L27" s="134" t="s">
-        <v>460</v>
+        <v>451</v>
       </c>
       <c r="M27" s="111" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="N27" s="109" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="O27" s="109" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="P27" s="109" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="Q27" s="109"/>
       <c r="R27" s="109" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="S27" s="111" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="T27" s="111" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="U27" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="V27" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="W27" s="111" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="X27" s="109" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="Y27" s="114">
         <v>400</v>
@@ -13166,14 +13166,14 @@
         <v>10000</v>
       </c>
       <c r="AA27" s="111" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="AB27" s="114" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="AC27" s="114"/>
       <c r="AD27" s="116" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="AE27" s="111"/>
       <c r="AF27" s="111"/>
@@ -13182,10 +13182,10 @@
     </row>
     <row r="28" spans="1:47" s="105" customFormat="1" ht="14.5" customHeight="1" thickBot="1">
       <c r="A28" s="145" t="s">
-        <v>470</v>
+        <v>461</v>
       </c>
       <c r="B28" s="162" t="s">
-        <v>469</v>
+        <v>460</v>
       </c>
       <c r="C28" s="109">
         <v>0.05</v>
@@ -13194,20 +13194,20 @@
         <v>0.15</v>
       </c>
       <c r="E28" s="110" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="F28" s="109" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="G28" s="111">
         <v>0.5</v>
       </c>
       <c r="H28" s="111"/>
       <c r="I28" s="111" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="J28" s="111" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="K28" s="111">
         <v>2</v>
@@ -13216,7 +13216,7 @@
         <v>10</v>
       </c>
       <c r="M28" s="111" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="N28" s="109">
         <v>0.85</v>
@@ -13235,33 +13235,33 @@
       </c>
       <c r="S28" s="111"/>
       <c r="T28" s="111" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="U28" s="111"/>
       <c r="V28" s="111" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="W28" s="111"/>
       <c r="X28" s="109">
         <v>0</v>
       </c>
       <c r="Y28" s="114" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="Z28" s="114" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="AA28" s="116" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="AB28" s="115" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="AC28" s="115" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="AD28" s="116" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="AE28" s="111"/>
       <c r="AF28" s="111"/>
@@ -13270,7 +13270,7 @@
     </row>
     <row r="29" spans="1:47" s="105" customFormat="1" ht="29.5" customHeight="1" thickBot="1">
       <c r="A29" s="119" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="B29" s="119" t="s">
         <v>96</v>
@@ -13282,31 +13282,31 @@
         <v>0.3</v>
       </c>
       <c r="E29" s="117" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="F29" s="109" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="G29" s="111" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="H29" s="111" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
       <c r="I29" s="111" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
       <c r="J29" s="111" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
       <c r="K29" s="111">
         <v>2</v>
       </c>
       <c r="L29" s="134" t="s">
-        <v>460</v>
+        <v>451</v>
       </c>
       <c r="M29" s="111" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="N29" s="109">
         <v>0.85</v>
@@ -13320,22 +13320,22 @@
       <c r="Q29" s="109"/>
       <c r="R29" s="109"/>
       <c r="S29" s="111" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="T29" s="111" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="U29" s="111" t="s">
-        <v>455</v>
+        <v>446</v>
       </c>
       <c r="V29" s="111" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="W29" s="111" t="s">
-        <v>453</v>
+        <v>444</v>
       </c>
       <c r="X29" s="109" t="s">
-        <v>454</v>
+        <v>445</v>
       </c>
       <c r="Y29" s="114">
         <v>15</v>
@@ -13344,7 +13344,7 @@
         <v>60</v>
       </c>
       <c r="AA29" s="111" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="AB29" s="114">
         <v>0.01</v>
@@ -13353,10 +13353,10 @@
         <v>0.23</v>
       </c>
       <c r="AD29" s="116" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="AE29" s="111" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="AF29" s="111"/>
       <c r="AG29" s="111"/>
@@ -13364,10 +13364,10 @@
     </row>
     <row r="30" spans="1:47" s="105" customFormat="1" ht="21.5" customHeight="1" thickBot="1">
       <c r="A30" s="118" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="B30" s="157" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="C30" s="109">
         <v>0.06</v>
@@ -13376,31 +13376,31 @@
         <v>0.01</v>
       </c>
       <c r="E30" s="117" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="F30" s="117" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="G30" s="111" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="H30" s="111" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
       <c r="I30" s="111" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
       <c r="J30" s="111" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
       <c r="K30" s="111">
         <v>2</v>
       </c>
       <c r="L30" s="134" t="s">
-        <v>460</v>
+        <v>451</v>
       </c>
       <c r="M30" s="111" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="N30" s="109">
         <v>0.85</v>
@@ -13412,28 +13412,28 @@
         <v>0.5</v>
       </c>
       <c r="Q30" s="109" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="R30" s="109" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="S30" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="T30" s="111" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
       <c r="U30" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="V30" s="111" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
       <c r="W30" s="111" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
       <c r="X30" s="111" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
       <c r="Y30" s="114">
         <v>1500</v>
@@ -13442,19 +13442,19 @@
         <v>3000</v>
       </c>
       <c r="AA30" s="111" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="AB30" s="114" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="AC30" s="114">
         <v>1500</v>
       </c>
       <c r="AD30" s="116" t="s">
-        <v>452</v>
+        <v>443</v>
       </c>
       <c r="AE30" s="111" t="s">
-        <v>451</v>
+        <v>510</v>
       </c>
       <c r="AF30" s="111"/>
       <c r="AG30" s="111"/>
@@ -13462,7 +13462,7 @@
     </row>
     <row r="31" spans="1:47" s="107" customFormat="1" ht="21.5" customHeight="1" thickBot="1">
       <c r="A31" s="118" t="s">
-        <v>466</v>
+        <v>457</v>
       </c>
       <c r="B31" s="157"/>
       <c r="C31" s="109"/>
@@ -13472,17 +13472,17 @@
       <c r="G31" s="111"/>
       <c r="H31" s="111"/>
       <c r="I31" s="111" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="J31" s="111" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="K31" s="111"/>
       <c r="L31" s="111">
         <v>10</v>
       </c>
       <c r="M31" s="111" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="N31" s="109"/>
       <c r="O31" s="109"/>
@@ -13521,7 +13521,7 @@
     </row>
     <row r="32" spans="1:47" s="107" customFormat="1" ht="21.5" customHeight="1" thickBot="1">
       <c r="A32" s="118" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
       <c r="B32" s="157"/>
       <c r="C32" s="109"/>
@@ -13652,14 +13652,14 @@
       </c>
       <c r="B35" s="162"/>
       <c r="C35" s="109" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="D35" s="109" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="E35" s="111"/>
       <c r="F35" s="109" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="G35" s="111"/>
       <c r="H35" s="111"/>
@@ -13686,7 +13686,7 @@
         <v>600</v>
       </c>
       <c r="AA35" s="111" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="AB35" s="114">
         <v>2.78</v>
@@ -13695,10 +13695,10 @@
         <v>13.89</v>
       </c>
       <c r="AD35" s="116" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="AE35" s="111" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="AF35" s="111"/>
       <c r="AG35" s="111"/>
@@ -13716,69 +13716,69 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="E36" s="111" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="F36" s="111" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="G36" s="111" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="H36" s="111" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="I36" s="111" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="J36" s="111" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="K36" s="111" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="L36" s="111" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="M36" s="111" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="N36" s="109">
         <v>0.72</v>
       </c>
       <c r="O36" s="109" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="P36" s="109" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="Q36" s="109"/>
       <c r="R36" s="109">
         <v>0.93</v>
       </c>
       <c r="S36" s="111" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="T36" s="111"/>
       <c r="U36" s="111" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="V36" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="W36" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="X36" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="Y36" s="114" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="Z36" s="114"/>
       <c r="AA36" s="111"/>
       <c r="AB36" s="114"/>
       <c r="AC36" s="114" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="AD36" s="116"/>
       <c r="AE36" s="111"/>
@@ -13792,10 +13792,10 @@
       </c>
       <c r="B37" s="157"/>
       <c r="C37" s="109" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="D37" s="109" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="E37" s="111"/>
       <c r="F37" s="111"/>
@@ -13834,7 +13834,7 @@
       </c>
       <c r="B38" s="157"/>
       <c r="C38" s="109" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="D38" s="111"/>
       <c r="E38" s="111"/>
@@ -13854,16 +13854,16 @@
       <c r="S38" s="111"/>
       <c r="T38" s="111"/>
       <c r="U38" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="V38" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="W38" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="X38" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="Y38" s="114">
         <v>9</v>
@@ -13872,7 +13872,7 @@
         <v>156</v>
       </c>
       <c r="AA38" s="111" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="AB38" s="114">
         <v>0</v>
@@ -13881,10 +13881,10 @@
         <v>0.2</v>
       </c>
       <c r="AD38" s="116" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="AE38" s="111" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="AF38" s="111"/>
       <c r="AG38" s="111"/>
@@ -13908,33 +13908,33 @@
         <v>16</v>
       </c>
       <c r="B39" s="165" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="C39" s="135">
         <v>0.02</v>
       </c>
       <c r="D39" s="135" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="E39" s="136"/>
       <c r="F39" s="136"/>
       <c r="G39" s="136" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="H39" s="136" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="I39" s="136" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="J39" s="136" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="K39" s="136" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="L39" s="136" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="M39" s="136"/>
       <c r="N39" s="137"/>
@@ -13942,23 +13942,23 @@
       <c r="P39" s="136"/>
       <c r="Q39" s="136"/>
       <c r="R39" s="136" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="S39" s="136"/>
       <c r="T39" s="136" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="U39" s="136" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="V39" s="136" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="W39" s="136" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="X39" s="136" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="Y39" s="138">
         <v>0.72</v>
@@ -13967,7 +13967,7 @@
         <v>2.54</v>
       </c>
       <c r="AA39" s="140" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="AB39" s="139">
         <v>0</v>
@@ -13976,10 +13976,10 @@
         <v>0</v>
       </c>
       <c r="AD39" s="140" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="AE39" s="136" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="AF39" s="111"/>
       <c r="AG39" s="111"/>
@@ -14001,33 +14001,33 @@
     <row r="40" spans="1:47" s="103" customFormat="1" ht="17" thickBot="1">
       <c r="A40" s="199"/>
       <c r="B40" s="166" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="C40" s="131" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="D40" s="131" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="E40" s="131"/>
       <c r="F40" s="131"/>
       <c r="G40" s="131" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="H40" s="131" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="I40" s="131" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="J40" s="131" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="K40" s="131" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="L40" s="131" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="M40" s="131"/>
       <c r="N40" s="130"/>
@@ -14035,23 +14035,23 @@
       <c r="P40" s="131"/>
       <c r="Q40" s="131"/>
       <c r="R40" s="131" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="S40" s="131"/>
       <c r="T40" s="131" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="U40" s="131" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="V40" s="131" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="W40" s="131" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="X40" s="131" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="Y40" s="141">
         <v>0.61</v>
@@ -14060,7 +14060,7 @@
         <v>2.88</v>
       </c>
       <c r="AA40" s="143" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="AB40" s="142">
         <v>0</v>
@@ -14069,10 +14069,10 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="AD40" s="143" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="AE40" s="131" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="AF40" s="111"/>
       <c r="AG40" s="111"/>
@@ -14096,7 +14096,7 @@
         <v>28</v>
       </c>
       <c r="B41" s="161" t="s">
-        <v>501</v>
+        <v>492</v>
       </c>
       <c r="C41" s="109">
         <v>0.02</v>
@@ -14105,7 +14105,7 @@
         <v>0.02</v>
       </c>
       <c r="E41" s="111" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="F41" s="109">
         <v>7.0000000000000007E-2</v>
@@ -14113,16 +14113,16 @@
       <c r="G41" s="111"/>
       <c r="H41" s="111"/>
       <c r="I41" s="111" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="J41" s="111" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="K41" s="111">
         <v>2</v>
       </c>
       <c r="L41" s="111" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="M41" s="111">
         <v>50</v>
@@ -14135,16 +14135,16 @@
       <c r="S41" s="111"/>
       <c r="T41" s="111"/>
       <c r="U41" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="V41" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="W41" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="X41" s="111" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="Y41" s="114">
         <v>0.55000000000000004</v>
@@ -14153,7 +14153,7 @@
         <v>24.52</v>
       </c>
       <c r="AA41" s="116" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="AB41" s="115">
         <v>0.04</v>
@@ -14162,10 +14162,10 @@
         <v>1</v>
       </c>
       <c r="AD41" s="116" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="AE41" s="111" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="AF41" s="111"/>
       <c r="AG41" s="111"/>
@@ -14187,7 +14187,7 @@
     <row r="42" spans="1:47" s="103" customFormat="1" ht="17" thickBot="1">
       <c r="A42" s="200"/>
       <c r="B42" s="159" t="s">
-        <v>502</v>
+        <v>493</v>
       </c>
       <c r="C42" s="109">
         <v>0.02</v>
@@ -14196,28 +14196,28 @@
         <v>0.02</v>
       </c>
       <c r="E42" s="111" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="F42" s="109">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="G42" s="111" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="H42" s="111" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="I42" s="111" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="J42" s="111" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="K42" s="111">
         <v>2</v>
       </c>
       <c r="L42" s="111" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="M42" s="111">
         <v>50</v>
@@ -14230,16 +14230,16 @@
       <c r="S42" s="111"/>
       <c r="T42" s="111"/>
       <c r="U42" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="V42" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="W42" s="111" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="X42" s="111" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="Y42" s="114"/>
       <c r="Z42" s="115"/>

</xml_diff>

<commit_message>
small tweaks, add back 1.42 conv factor
</commit_message>
<xml_diff>
--- a/data/ResearchProjectSpreadsheet_ReadForm.xlsx
+++ b/data/ResearchProjectSpreadsheet_ReadForm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daxledesma/Documents/GitHub/tdot-gi-streamlit/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07B185CB-5842-BF4C-8CED-2AD2A2E0C7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7DC1BB-8FB7-6846-B904-968586D7F50D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-21600" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{B220E2DF-F534-4A75-BFA7-DDC35956FE64}"/>
+    <workbookView xWindow="1260" yWindow="0" windowWidth="37140" windowHeight="21600" activeTab="4" xr2:uid="{B220E2DF-F534-4A75-BFA7-DDC35956FE64}"/>
   </bookViews>
   <sheets>
     <sheet name="GI" sheetId="5" r:id="rId1"/>
@@ -1608,22 +1608,22 @@
     <t>0-10</t>
   </si>
   <si>
-    <t>Total Suspended Solids (TSS) (Minimum required)</t>
-  </si>
-  <si>
-    <t>Total Phosphorous (TP) (Minimum required)</t>
-  </si>
-  <si>
-    <t>Total Nitrogen (TN) (Minimum required)</t>
-  </si>
-  <si>
-    <t>Metals (Minimum required)</t>
-  </si>
-  <si>
-    <t>Organism removal (Minimum required)</t>
-  </si>
-  <si>
     <t>Indefinitely</t>
+  </si>
+  <si>
+    <t>Total Suspended Solids (TSS) (%; Minimum required)</t>
+  </si>
+  <si>
+    <t>Total Phosphorous (TP) (%; Minimum required)</t>
+  </si>
+  <si>
+    <t>Total Nitrogen (TN) (%; Minimum required)</t>
+  </si>
+  <si>
+    <t>Metals (%; Minimum required)</t>
+  </si>
+  <si>
+    <t>Organism removal (%; Minimum required)</t>
   </si>
 </sst>
 </file>
@@ -2769,30 +2769,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2819,40 +2840,73 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2881,60 +2935,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3318,39 +3318,39 @@
     </row>
     <row r="2" spans="1:38" ht="17" thickBot="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="171" t="s">
+      <c r="B2" s="168" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="171" t="s">
+      <c r="C2" s="168" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="181" t="s">
+      <c r="D2" s="188" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="171" t="s">
+      <c r="E2" s="168" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="171" t="s">
+      <c r="G2" s="168" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="174" t="s">
+      <c r="H2" s="182" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="190" t="s">
+      <c r="I2" s="179" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="191"/>
-      <c r="K2" s="192"/>
-      <c r="L2" s="171" t="s">
+      <c r="J2" s="180"/>
+      <c r="K2" s="181"/>
+      <c r="L2" s="168" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="171" t="s">
+      <c r="M2" s="168" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="171" t="s">
+      <c r="N2" s="168" t="s">
         <v>11</v>
       </c>
       <c r="O2" s="1"/>
@@ -3380,15 +3380,15 @@
     </row>
     <row r="3" spans="1:38" ht="17" thickBot="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="175"/>
-      <c r="C3" s="175"/>
-      <c r="D3" s="182"/>
-      <c r="E3" s="170"/>
+      <c r="B3" s="169"/>
+      <c r="C3" s="169"/>
+      <c r="D3" s="189"/>
+      <c r="E3" s="171"/>
       <c r="F3" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="170"/>
-      <c r="H3" s="170"/>
+      <c r="G3" s="171"/>
+      <c r="H3" s="171"/>
       <c r="I3" s="23" t="s">
         <v>13</v>
       </c>
@@ -3398,9 +3398,9 @@
       <c r="K3" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="175"/>
-      <c r="M3" s="175"/>
-      <c r="N3" s="189"/>
+      <c r="L3" s="169"/>
+      <c r="M3" s="169"/>
+      <c r="N3" s="178"/>
       <c r="O3" s="81"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
@@ -3478,7 +3478,7 @@
     </row>
     <row r="5" spans="1:38" ht="15" customHeight="1" thickBot="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="177" t="s">
+      <c r="B5" s="184" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -3500,7 +3500,7 @@
       <c r="K5" s="12"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
-      <c r="N5" s="168" t="s">
+      <c r="N5" s="170" t="s">
         <v>20</v>
       </c>
       <c r="O5" s="1"/>
@@ -3530,7 +3530,7 @@
     </row>
     <row r="6" spans="1:38" ht="15" customHeight="1" thickBot="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="177"/>
+      <c r="B6" s="184"/>
       <c r="C6" s="8" t="s">
         <v>25</v>
       </c>
@@ -3550,7 +3550,7 @@
       <c r="K6" s="14"/>
       <c r="L6" s="18"/>
       <c r="M6" s="18"/>
-      <c r="N6" s="170"/>
+      <c r="N6" s="171"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
@@ -3578,7 +3578,7 @@
     </row>
     <row r="7" spans="1:38" ht="15" customHeight="1" thickBot="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="176" t="s">
+      <c r="B7" s="183" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="6" t="s">
@@ -3600,7 +3600,7 @@
       <c r="K7" s="12"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
-      <c r="N7" s="168" t="s">
+      <c r="N7" s="170" t="s">
         <v>33</v>
       </c>
       <c r="O7" s="1"/>
@@ -3630,7 +3630,7 @@
     </row>
     <row r="8" spans="1:38" ht="15" customHeight="1" thickBot="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="177"/>
+      <c r="B8" s="184"/>
       <c r="C8" s="8" t="s">
         <v>34</v>
       </c>
@@ -3650,7 +3650,7 @@
       <c r="K8" s="14"/>
       <c r="L8" s="18"/>
       <c r="M8" s="18"/>
-      <c r="N8" s="170"/>
+      <c r="N8" s="171"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
@@ -3678,7 +3678,7 @@
     </row>
     <row r="9" spans="1:38" ht="15" customHeight="1" thickBot="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="188" t="s">
+      <c r="B9" s="177" t="s">
         <v>37</v>
       </c>
       <c r="C9" s="24" t="s">
@@ -3730,7 +3730,7 @@
     </row>
     <row r="10" spans="1:38" ht="15" customHeight="1" thickBot="1">
       <c r="A10" s="1"/>
-      <c r="B10" s="173"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="89" t="s">
         <v>41</v>
       </c>
@@ -3794,7 +3794,7 @@
       <c r="K11" s="92"/>
       <c r="L11" s="91"/>
       <c r="M11" s="91"/>
-      <c r="N11" s="168">
+      <c r="N11" s="170">
         <v>5</v>
       </c>
       <c r="O11" s="1"/>
@@ -3824,7 +3824,7 @@
     </row>
     <row r="12" spans="1:38" ht="15" customHeight="1" thickBot="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="173"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="89" t="s">
         <v>45</v>
       </c>
@@ -3840,7 +3840,7 @@
       <c r="K12" s="92"/>
       <c r="L12" s="91"/>
       <c r="M12" s="91"/>
-      <c r="N12" s="170"/>
+      <c r="N12" s="171"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
@@ -3914,7 +3914,7 @@
     </row>
     <row r="14" spans="1:38" ht="16.25" customHeight="1" thickBot="1">
       <c r="A14" s="1"/>
-      <c r="B14" s="178" t="s">
+      <c r="B14" s="185" t="s">
         <v>47</v>
       </c>
       <c r="C14" s="41" t="s">
@@ -3936,7 +3936,7 @@
       <c r="K14" s="29"/>
       <c r="L14" s="28"/>
       <c r="M14" s="5"/>
-      <c r="N14" s="168" t="s">
+      <c r="N14" s="170" t="s">
         <v>51</v>
       </c>
       <c r="O14" s="1"/>
@@ -3966,7 +3966,7 @@
     </row>
     <row r="15" spans="1:38" ht="15" customHeight="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="179"/>
+      <c r="B15" s="186"/>
       <c r="C15" s="7" t="s">
         <v>52</v>
       </c>
@@ -3986,7 +3986,7 @@
       <c r="K15" s="13"/>
       <c r="L15" s="17"/>
       <c r="M15" s="17"/>
-      <c r="N15" s="169"/>
+      <c r="N15" s="176"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
@@ -4014,7 +4014,7 @@
     </row>
     <row r="16" spans="1:38" ht="15" customHeight="1" thickBot="1">
       <c r="A16" s="1"/>
-      <c r="B16" s="179"/>
+      <c r="B16" s="186"/>
       <c r="C16" s="7" t="s">
         <v>54</v>
       </c>
@@ -4034,7 +4034,7 @@
       <c r="K16" s="13"/>
       <c r="L16" s="17"/>
       <c r="M16" s="17"/>
-      <c r="N16" s="169"/>
+      <c r="N16" s="176"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
@@ -4062,7 +4062,7 @@
     </row>
     <row r="17" spans="1:38" ht="33" customHeight="1" thickBot="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="180"/>
+      <c r="B17" s="187"/>
       <c r="C17" s="75" t="s">
         <v>57</v>
       </c>
@@ -4082,7 +4082,7 @@
       <c r="K17" s="14"/>
       <c r="L17" s="18"/>
       <c r="M17" s="18"/>
-      <c r="N17" s="170"/>
+      <c r="N17" s="171"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
@@ -4182,7 +4182,7 @@
       <c r="K19" s="12"/>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
-      <c r="N19" s="168" t="s">
+      <c r="N19" s="170" t="s">
         <v>67</v>
       </c>
       <c r="O19" s="1"/>
@@ -4212,7 +4212,7 @@
     </row>
     <row r="20" spans="1:38" ht="15" customHeight="1" thickBot="1">
       <c r="A20" s="1"/>
-      <c r="B20" s="173"/>
+      <c r="B20" s="174"/>
       <c r="C20" s="8" t="s">
         <v>68</v>
       </c>
@@ -4232,7 +4232,7 @@
       <c r="K20" s="14"/>
       <c r="L20" s="18"/>
       <c r="M20" s="18"/>
-      <c r="N20" s="170"/>
+      <c r="N20" s="171"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
@@ -4278,7 +4278,7 @@
       <c r="K21" s="38"/>
       <c r="L21" s="36"/>
       <c r="M21" s="36"/>
-      <c r="N21" s="187">
+      <c r="N21" s="175">
         <v>5</v>
       </c>
       <c r="O21" s="1"/>
@@ -4308,7 +4308,7 @@
     </row>
     <row r="22" spans="1:38" ht="15" customHeight="1" thickBot="1">
       <c r="A22" s="1"/>
-      <c r="B22" s="186"/>
+      <c r="B22" s="173"/>
       <c r="C22" s="35" t="s">
         <v>72</v>
       </c>
@@ -4324,7 +4324,7 @@
       <c r="K22" s="38"/>
       <c r="L22" s="36"/>
       <c r="M22" s="36"/>
-      <c r="N22" s="169"/>
+      <c r="N22" s="176"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
@@ -4352,7 +4352,7 @@
     </row>
     <row r="23" spans="1:38" ht="15" customHeight="1" thickBot="1">
       <c r="A23" s="1"/>
-      <c r="B23" s="173"/>
+      <c r="B23" s="174"/>
       <c r="C23" s="35" t="s">
         <v>45</v>
       </c>
@@ -4368,7 +4368,7 @@
       <c r="K23" s="38"/>
       <c r="L23" s="36"/>
       <c r="M23" s="36"/>
-      <c r="N23" s="170"/>
+      <c r="N23" s="171"/>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
@@ -4693,10 +4693,10 @@
       <c r="C30" s="87" t="s">
         <v>88</v>
       </c>
-      <c r="D30" s="183" t="s">
+      <c r="D30" s="190" t="s">
         <v>89</v>
       </c>
-      <c r="E30" s="184"/>
+      <c r="E30" s="191"/>
       <c r="F30" s="79" t="s">
         <v>44</v>
       </c>
@@ -4714,12 +4714,12 @@
       </c>
     </row>
     <row r="31" spans="1:38" ht="25.25" customHeight="1" thickBot="1">
-      <c r="B31" s="173"/>
+      <c r="B31" s="174"/>
       <c r="C31" s="87" t="s">
         <v>91</v>
       </c>
-      <c r="D31" s="173"/>
-      <c r="E31" s="185"/>
+      <c r="D31" s="174"/>
+      <c r="E31" s="192"/>
       <c r="F31" s="79" t="s">
         <v>44</v>
       </c>
@@ -4971,7 +4971,7 @@
       <c r="AL36" s="1"/>
     </row>
     <row r="37" spans="1:38" ht="15" customHeight="1" thickBot="1">
-      <c r="A37" s="168" t="s">
+      <c r="A37" s="170" t="s">
         <v>101</v>
       </c>
       <c r="B37" s="47" t="s">
@@ -5021,7 +5021,7 @@
       <c r="AL37" s="1"/>
     </row>
     <row r="38" spans="1:38" ht="15" customHeight="1" thickBot="1">
-      <c r="A38" s="169"/>
+      <c r="A38" s="176"/>
       <c r="B38" s="47" t="s">
         <v>104</v>
       </c>
@@ -5069,7 +5069,7 @@
       <c r="AL38" s="1"/>
     </row>
     <row r="39" spans="1:38" ht="15" customHeight="1" thickBot="1">
-      <c r="A39" s="169"/>
+      <c r="A39" s="176"/>
       <c r="B39" s="47" t="s">
         <v>106</v>
       </c>
@@ -5117,7 +5117,7 @@
       <c r="AL39" s="1"/>
     </row>
     <row r="40" spans="1:38" ht="15" customHeight="1" thickBot="1">
-      <c r="A40" s="169"/>
+      <c r="A40" s="176"/>
       <c r="B40" s="47" t="s">
         <v>108</v>
       </c>
@@ -5165,7 +5165,7 @@
       <c r="AL40" s="1"/>
     </row>
     <row r="41" spans="1:38" ht="15" customHeight="1" thickBot="1">
-      <c r="A41" s="169"/>
+      <c r="A41" s="176"/>
       <c r="B41" s="47" t="s">
         <v>110</v>
       </c>
@@ -5213,7 +5213,7 @@
       <c r="AL41" s="1"/>
     </row>
     <row r="42" spans="1:38" ht="15" customHeight="1" thickBot="1">
-      <c r="A42" s="170"/>
+      <c r="A42" s="171"/>
       <c r="B42" s="47" t="s">
         <v>112</v>
       </c>
@@ -8601,19 +8601,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="N21:N23"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="N14:N17"/>
-    <mergeCell ref="N19:N20"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="I2:K2"/>
-    <mergeCell ref="L2:L3"/>
     <mergeCell ref="A37:A42"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="B19:B20"/>
@@ -8628,6 +8615,19 @@
     <mergeCell ref="B30:B31"/>
     <mergeCell ref="D30:D31"/>
     <mergeCell ref="E30:E31"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="N21:N23"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="N14:N17"/>
+    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="L2:L3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9564,33 +9564,33 @@
     </row>
     <row r="2" spans="1:17" ht="16" thickBot="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="171" t="s">
+      <c r="B2" s="168" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="171" t="s">
+      <c r="C2" s="168" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="194" t="s">
+      <c r="D2" s="193" t="s">
         <v>291</v>
       </c>
-      <c r="E2" s="195"/>
-      <c r="F2" s="196"/>
-      <c r="G2" s="196"/>
-      <c r="H2" s="196"/>
-      <c r="I2" s="196"/>
-      <c r="J2" s="196"/>
-      <c r="K2" s="196"/>
-      <c r="L2" s="196"/>
-      <c r="M2" s="196"/>
-      <c r="N2" s="196"/>
-      <c r="O2" s="196"/>
-      <c r="P2" s="196"/>
-      <c r="Q2" s="197"/>
+      <c r="E2" s="194"/>
+      <c r="F2" s="195"/>
+      <c r="G2" s="195"/>
+      <c r="H2" s="195"/>
+      <c r="I2" s="195"/>
+      <c r="J2" s="195"/>
+      <c r="K2" s="195"/>
+      <c r="L2" s="195"/>
+      <c r="M2" s="195"/>
+      <c r="N2" s="195"/>
+      <c r="O2" s="195"/>
+      <c r="P2" s="195"/>
+      <c r="Q2" s="196"/>
     </row>
     <row r="3" spans="1:17" ht="16" thickBot="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="175"/>
-      <c r="C3" s="175"/>
+      <c r="B3" s="169"/>
+      <c r="C3" s="169"/>
       <c r="D3" s="83" t="s">
         <v>292</v>
       </c>
@@ -9664,7 +9664,7 @@
     </row>
     <row r="5" spans="1:17" ht="16" thickBot="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="177" t="str">
+      <c r="B5" s="184" t="str">
         <f>GI!B5</f>
         <v>Rain Garden</v>
       </c>
@@ -9672,7 +9672,7 @@
         <f>GI!C5</f>
         <v>bioretention/bioinfiltration</v>
       </c>
-      <c r="D5" s="168" t="str">
+      <c r="D5" s="170" t="str">
         <f>GI!N5</f>
         <v>1,2,4</v>
       </c>
@@ -9692,12 +9692,12 @@
     </row>
     <row r="6" spans="1:17" ht="16" thickBot="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="177"/>
+      <c r="B6" s="184"/>
       <c r="C6" s="8" t="str">
         <f>GI!C6</f>
         <v>bioretention cells</v>
       </c>
-      <c r="D6" s="193"/>
+      <c r="D6" s="197"/>
       <c r="E6" s="97"/>
       <c r="F6" s="43"/>
       <c r="G6" s="43"/>
@@ -9714,7 +9714,7 @@
     </row>
     <row r="7" spans="1:17" ht="16" thickBot="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="176" t="str">
+      <c r="B7" s="183" t="str">
         <f>GI!B7</f>
         <v>Planter Boxes</v>
       </c>
@@ -9722,7 +9722,7 @@
         <f>GI!C7</f>
         <v>open bottom</v>
       </c>
-      <c r="D7" s="168" t="str">
+      <c r="D7" s="170" t="str">
         <f>GI!N7</f>
         <v>1,2</v>
       </c>
@@ -9742,12 +9742,12 @@
     </row>
     <row r="8" spans="1:17" ht="16" thickBot="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="177"/>
+      <c r="B8" s="184"/>
       <c r="C8" s="8" t="str">
         <f>GI!C8</f>
         <v>closed bottom</v>
       </c>
-      <c r="D8" s="193"/>
+      <c r="D8" s="197"/>
       <c r="E8" s="97"/>
       <c r="F8" s="43"/>
       <c r="G8" s="43"/>
@@ -9764,7 +9764,7 @@
     </row>
     <row r="9" spans="1:17" ht="16" thickBot="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="188" t="str">
+      <c r="B9" s="177" t="str">
         <f>GI!B9</f>
         <v>Bioretention Areas</v>
       </c>
@@ -9792,7 +9792,7 @@
     </row>
     <row r="10" spans="1:17" ht="16" thickBot="1">
       <c r="A10" s="1"/>
-      <c r="B10" s="173"/>
+      <c r="B10" s="174"/>
       <c r="C10" s="89" t="str">
         <f>GI!C10</f>
         <v>Bioslopes</v>
@@ -9827,7 +9827,7 @@
         <f>GI!C11</f>
         <v>w/ open underdrain</v>
       </c>
-      <c r="D11" s="168">
+      <c r="D11" s="170">
         <f>GI!N11</f>
         <v>5</v>
       </c>
@@ -9849,12 +9849,12 @@
     </row>
     <row r="12" spans="1:17" ht="16" thickBot="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="173"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="89" t="str">
         <f>GI!C12</f>
         <v>w/ capped underdrain</v>
       </c>
-      <c r="D12" s="193"/>
+      <c r="D12" s="197"/>
       <c r="E12" s="97"/>
       <c r="F12" s="43"/>
       <c r="G12" s="43"/>
@@ -9903,7 +9903,7 @@
     </row>
     <row r="14" spans="1:17">
       <c r="A14" s="1"/>
-      <c r="B14" s="178" t="str">
+      <c r="B14" s="185" t="str">
         <f>GI!B14</f>
         <v>Permeable Pavements</v>
       </c>
@@ -9911,7 +9911,7 @@
         <f>GI!C14</f>
         <v>pervious concrete</v>
       </c>
-      <c r="D14" s="168" t="str">
+      <c r="D14" s="170" t="str">
         <f>GI!N14</f>
         <v>1,2,3,4</v>
       </c>
@@ -9931,12 +9931,12 @@
     </row>
     <row r="15" spans="1:17">
       <c r="A15" s="1"/>
-      <c r="B15" s="179"/>
+      <c r="B15" s="186"/>
       <c r="C15" s="7" t="str">
         <f>GI!C15</f>
         <v>pervious asphalt</v>
       </c>
-      <c r="D15" s="175"/>
+      <c r="D15" s="169"/>
       <c r="E15" s="97"/>
       <c r="F15" s="43"/>
       <c r="G15" s="43"/>
@@ -9953,12 +9953,12 @@
     </row>
     <row r="16" spans="1:17">
       <c r="A16" s="1"/>
-      <c r="B16" s="179"/>
+      <c r="B16" s="186"/>
       <c r="C16" s="7" t="str">
         <f>GI!C16</f>
         <v>pervious pavers</v>
       </c>
-      <c r="D16" s="175"/>
+      <c r="D16" s="169"/>
       <c r="E16" s="97"/>
       <c r="F16" s="43"/>
       <c r="G16" s="43"/>
@@ -9975,12 +9975,12 @@
     </row>
     <row r="17" spans="1:17" ht="16" thickBot="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="180"/>
+      <c r="B17" s="187"/>
       <c r="C17" s="75" t="str">
         <f>GI!C17</f>
         <v>permiable interlocking pavers</v>
       </c>
-      <c r="D17" s="193"/>
+      <c r="D17" s="197"/>
       <c r="E17" s="97"/>
       <c r="F17" s="43"/>
       <c r="G17" s="43"/>
@@ -10033,7 +10033,7 @@
         <f>GI!C19</f>
         <v>dry detention basin</v>
       </c>
-      <c r="D19" s="168" t="str">
+      <c r="D19" s="170" t="str">
         <f>GI!N19</f>
         <v>4, 5</v>
       </c>
@@ -10055,12 +10055,12 @@
     </row>
     <row r="20" spans="1:17" ht="16" thickBot="1">
       <c r="A20" s="1"/>
-      <c r="B20" s="173"/>
+      <c r="B20" s="174"/>
       <c r="C20" s="8" t="str">
         <f>GI!C20</f>
         <v>wet detention basin</v>
       </c>
-      <c r="D20" s="193"/>
+      <c r="D20" s="197"/>
       <c r="E20" s="97"/>
       <c r="F20" s="43"/>
       <c r="G20" s="43"/>
@@ -10087,7 +10087,7 @@
         <f>GI!C21</f>
         <v>w/ open underdrain</v>
       </c>
-      <c r="D21" s="187">
+      <c r="D21" s="175">
         <f>GI!N21</f>
         <v>5</v>
       </c>
@@ -10107,12 +10107,12 @@
     </row>
     <row r="22" spans="1:17" ht="16" thickBot="1">
       <c r="A22" s="1"/>
-      <c r="B22" s="186"/>
+      <c r="B22" s="173"/>
       <c r="C22" s="35" t="str">
         <f>GI!C22</f>
         <v>w/ upturned underdrain</v>
       </c>
-      <c r="D22" s="169"/>
+      <c r="D22" s="176"/>
       <c r="E22" s="97"/>
       <c r="F22" s="43"/>
       <c r="G22" s="43"/>
@@ -10129,12 +10129,12 @@
     </row>
     <row r="23" spans="1:17" ht="16" thickBot="1">
       <c r="A23" s="1"/>
-      <c r="B23" s="173"/>
+      <c r="B23" s="174"/>
       <c r="C23" s="35" t="str">
         <f>GI!C23</f>
         <v>w/ capped underdrain</v>
       </c>
-      <c r="D23" s="170"/>
+      <c r="D23" s="171"/>
       <c r="E23" s="97"/>
       <c r="F23" s="43"/>
       <c r="G23" s="43"/>
@@ -10345,7 +10345,7 @@
       <c r="Q30" s="43"/>
     </row>
     <row r="31" spans="1:17" ht="16" thickBot="1">
-      <c r="B31" s="173"/>
+      <c r="B31" s="174"/>
       <c r="C31" s="87" t="str">
         <f>GI!C31</f>
         <v>Level 1</v>
@@ -10509,7 +10509,7 @@
       <c r="Q36" s="43"/>
     </row>
     <row r="37" spans="1:17" ht="16" thickBot="1">
-      <c r="A37" s="168" t="s">
+      <c r="A37" s="170" t="s">
         <v>101</v>
       </c>
       <c r="B37" s="47" t="str">
@@ -10539,7 +10539,7 @@
       <c r="Q37" s="43"/>
     </row>
     <row r="38" spans="1:17" ht="16" thickBot="1">
-      <c r="A38" s="169"/>
+      <c r="A38" s="176"/>
       <c r="B38" s="47" t="str">
         <f>GI!B38</f>
         <v>Green Parking</v>
@@ -10567,7 +10567,7 @@
       <c r="Q38" s="43"/>
     </row>
     <row r="39" spans="1:17" ht="16" thickBot="1">
-      <c r="A39" s="169"/>
+      <c r="A39" s="176"/>
       <c r="B39" s="47" t="str">
         <f>GI!B39</f>
         <v>Green Roofs</v>
@@ -10595,7 +10595,7 @@
       <c r="Q39" s="43"/>
     </row>
     <row r="40" spans="1:17" ht="16" thickBot="1">
-      <c r="A40" s="169"/>
+      <c r="A40" s="176"/>
       <c r="B40" s="47" t="str">
         <f>GI!B40</f>
         <v>Urban Tree Canopy</v>
@@ -10623,7 +10623,7 @@
       <c r="Q40" s="43"/>
     </row>
     <row r="41" spans="1:17" ht="16" thickBot="1">
-      <c r="A41" s="169"/>
+      <c r="A41" s="176"/>
       <c r="B41" s="47" t="str">
         <f>GI!B41</f>
         <v>Land Conservation</v>
@@ -10651,7 +10651,7 @@
       <c r="Q41" s="43"/>
     </row>
     <row r="42" spans="1:17" ht="16" thickBot="1">
-      <c r="A42" s="170"/>
+      <c r="A42" s="171"/>
       <c r="B42" s="47" t="str">
         <f>GI!B42</f>
         <v>Downspout Disconnect</v>
@@ -10680,12 +10680,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="D2:Q2"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
     <mergeCell ref="B30:B31"/>
     <mergeCell ref="A37:A42"/>
     <mergeCell ref="D5:D6"/>
@@ -10698,6 +10692,12 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="D19:D20"/>
     <mergeCell ref="D21:D23"/>
+    <mergeCell ref="D2:Q2"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I13" r:id="rId1" location="page=50" xr:uid="{EB5A25CA-ECC4-4A9D-8F72-4681D3CC197D}"/>
@@ -10717,8 +10717,8 @@
   <dimension ref="A1:AU62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="75" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="W1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AE30" sqref="AE30"/>
+      <pane xSplit="1" topLeftCell="T1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -10797,83 +10797,83 @@
     </row>
     <row r="2" spans="1:47" ht="17.5" customHeight="1">
       <c r="A2" s="122"/>
-      <c r="B2" s="221" t="s">
+      <c r="B2" s="201" t="s">
         <v>491</v>
       </c>
-      <c r="C2" s="212" t="s">
+      <c r="C2" s="198" t="s">
         <v>304</v>
       </c>
-      <c r="D2" s="213"/>
-      <c r="E2" s="213"/>
-      <c r="F2" s="214"/>
-      <c r="G2" s="212" t="s">
+      <c r="D2" s="199"/>
+      <c r="E2" s="199"/>
+      <c r="F2" s="200"/>
+      <c r="G2" s="198" t="s">
         <v>471</v>
       </c>
-      <c r="H2" s="213"/>
-      <c r="I2" s="213"/>
-      <c r="J2" s="213"/>
-      <c r="K2" s="213"/>
-      <c r="L2" s="213" t="s">
+      <c r="H2" s="199"/>
+      <c r="I2" s="199"/>
+      <c r="J2" s="199"/>
+      <c r="K2" s="199"/>
+      <c r="L2" s="199" t="s">
         <v>472</v>
       </c>
-      <c r="M2" s="214"/>
-      <c r="N2" s="212" t="s">
+      <c r="M2" s="200"/>
+      <c r="N2" s="198" t="s">
         <v>473</v>
       </c>
-      <c r="O2" s="213"/>
-      <c r="P2" s="213"/>
-      <c r="Q2" s="213"/>
-      <c r="R2" s="214"/>
-      <c r="S2" s="211" t="s">
+      <c r="O2" s="199"/>
+      <c r="P2" s="199"/>
+      <c r="Q2" s="199"/>
+      <c r="R2" s="200"/>
+      <c r="S2" s="209" t="s">
         <v>469</v>
       </c>
-      <c r="T2" s="211"/>
-      <c r="U2" s="211"/>
-      <c r="V2" s="211"/>
-      <c r="W2" s="211"/>
-      <c r="X2" s="211"/>
-      <c r="Y2" s="211" t="s">
+      <c r="T2" s="209"/>
+      <c r="U2" s="209"/>
+      <c r="V2" s="209"/>
+      <c r="W2" s="209"/>
+      <c r="X2" s="209"/>
+      <c r="Y2" s="209" t="s">
         <v>303</v>
       </c>
-      <c r="Z2" s="211"/>
-      <c r="AA2" s="211"/>
-      <c r="AB2" s="211"/>
-      <c r="AC2" s="211"/>
-      <c r="AD2" s="211"/>
+      <c r="Z2" s="209"/>
+      <c r="AA2" s="209"/>
+      <c r="AB2" s="209"/>
+      <c r="AC2" s="209"/>
+      <c r="AD2" s="209"/>
       <c r="AE2" s="128" t="s">
         <v>338</v>
       </c>
-      <c r="AF2" s="212" t="s">
+      <c r="AF2" s="198" t="s">
         <v>116</v>
       </c>
-      <c r="AG2" s="213"/>
-      <c r="AH2" s="214"/>
+      <c r="AG2" s="199"/>
+      <c r="AH2" s="200"/>
     </row>
     <row r="3" spans="1:47" ht="28.75" customHeight="1">
       <c r="A3" s="108" t="s">
         <v>298</v>
       </c>
-      <c r="B3" s="222"/>
+      <c r="B3" s="202"/>
       <c r="C3" s="148" t="s">
         <v>362</v>
       </c>
       <c r="D3" s="148" t="s">
         <v>314</v>
       </c>
-      <c r="E3" s="217" t="s">
+      <c r="E3" s="207" t="s">
         <v>330</v>
       </c>
-      <c r="F3" s="219"/>
+      <c r="F3" s="208"/>
       <c r="G3" s="148" t="s">
         <v>323</v>
       </c>
       <c r="H3" s="148" t="s">
         <v>325</v>
       </c>
-      <c r="I3" s="217" t="s">
+      <c r="I3" s="207" t="s">
         <v>322</v>
       </c>
-      <c r="J3" s="219"/>
+      <c r="J3" s="208"/>
       <c r="K3" s="148" t="s">
         <v>335</v>
       </c>
@@ -10883,59 +10883,59 @@
       <c r="M3" s="148" t="s">
         <v>318</v>
       </c>
-      <c r="N3" s="215" t="s">
-        <v>505</v>
-      </c>
-      <c r="O3" s="215" t="s">
+      <c r="N3" s="205" t="s">
         <v>506</v>
       </c>
-      <c r="P3" s="215" t="s">
+      <c r="O3" s="205" t="s">
         <v>507</v>
       </c>
-      <c r="Q3" s="215" t="s">
+      <c r="P3" s="205" t="s">
         <v>508</v>
       </c>
-      <c r="R3" s="215" t="s">
+      <c r="Q3" s="205" t="s">
         <v>509</v>
       </c>
-      <c r="S3" s="220" t="s">
+      <c r="R3" s="205" t="s">
+        <v>510</v>
+      </c>
+      <c r="S3" s="210" t="s">
         <v>299</v>
       </c>
-      <c r="T3" s="220" t="s">
+      <c r="T3" s="210" t="s">
         <v>462</v>
       </c>
-      <c r="U3" s="220" t="s">
+      <c r="U3" s="210" t="s">
         <v>463</v>
       </c>
-      <c r="V3" s="220" t="s">
+      <c r="V3" s="210" t="s">
         <v>464</v>
       </c>
-      <c r="W3" s="220" t="s">
+      <c r="W3" s="210" t="s">
         <v>465</v>
       </c>
-      <c r="X3" s="220" t="s">
+      <c r="X3" s="210" t="s">
         <v>466</v>
       </c>
-      <c r="Y3" s="217" t="s">
+      <c r="Y3" s="207" t="s">
         <v>300</v>
       </c>
-      <c r="Z3" s="218"/>
-      <c r="AA3" s="219"/>
-      <c r="AB3" s="217" t="s">
+      <c r="Z3" s="215"/>
+      <c r="AA3" s="208"/>
+      <c r="AB3" s="207" t="s">
         <v>301</v>
       </c>
-      <c r="AC3" s="218"/>
-      <c r="AD3" s="218"/>
+      <c r="AC3" s="215"/>
+      <c r="AD3" s="215"/>
       <c r="AE3" s="147" t="s">
         <v>336</v>
       </c>
-      <c r="AF3" s="223" t="s">
+      <c r="AF3" s="203" t="s">
         <v>477</v>
       </c>
-      <c r="AG3" s="215" t="s">
+      <c r="AG3" s="205" t="s">
         <v>478</v>
       </c>
-      <c r="AH3" s="215" t="s">
+      <c r="AH3" s="205" t="s">
         <v>476</v>
       </c>
     </row>
@@ -10975,17 +10975,17 @@
       <c r="M4" s="150" t="s">
         <v>316</v>
       </c>
-      <c r="N4" s="216"/>
-      <c r="O4" s="216"/>
-      <c r="P4" s="216"/>
-      <c r="Q4" s="216"/>
-      <c r="R4" s="216"/>
-      <c r="S4" s="216"/>
-      <c r="T4" s="216"/>
-      <c r="U4" s="216"/>
-      <c r="V4" s="216"/>
-      <c r="W4" s="216"/>
-      <c r="X4" s="216"/>
+      <c r="N4" s="206"/>
+      <c r="O4" s="206"/>
+      <c r="P4" s="206"/>
+      <c r="Q4" s="206"/>
+      <c r="R4" s="206"/>
+      <c r="S4" s="206"/>
+      <c r="T4" s="206"/>
+      <c r="U4" s="206"/>
+      <c r="V4" s="206"/>
+      <c r="W4" s="206"/>
+      <c r="X4" s="206"/>
       <c r="Y4" s="151" t="s">
         <v>305</v>
       </c>
@@ -11007,12 +11007,12 @@
       <c r="AE4" s="146" t="s">
         <v>337</v>
       </c>
-      <c r="AF4" s="224"/>
-      <c r="AG4" s="216"/>
-      <c r="AH4" s="216"/>
+      <c r="AF4" s="204"/>
+      <c r="AG4" s="206"/>
+      <c r="AH4" s="206"/>
     </row>
     <row r="5" spans="1:47" s="107" customFormat="1" ht="15.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A5" s="198" t="s">
+      <c r="A5" s="216" t="s">
         <v>355</v>
       </c>
       <c r="B5" s="157" t="s">
@@ -11041,7 +11041,7 @@
       <c r="K5" s="111">
         <v>2</v>
       </c>
-      <c r="L5" s="209" t="s">
+      <c r="L5" s="213" t="s">
         <v>419</v>
       </c>
       <c r="M5" s="111">
@@ -11109,7 +11109,7 @@
       <c r="AU5" s="105"/>
     </row>
     <row r="6" spans="1:47" s="107" customFormat="1" ht="15" customHeight="1">
-      <c r="A6" s="201"/>
+      <c r="A6" s="219"/>
       <c r="B6" s="158" t="s">
         <v>41</v>
       </c>
@@ -11138,7 +11138,7 @@
       <c r="K6" s="111">
         <v>2</v>
       </c>
-      <c r="L6" s="210"/>
+      <c r="L6" s="214"/>
       <c r="M6" s="111" t="s">
         <v>450</v>
       </c>
@@ -11212,7 +11212,7 @@
       <c r="AU6" s="105"/>
     </row>
     <row r="7" spans="1:47" s="105" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A7" s="201"/>
+      <c r="A7" s="219"/>
       <c r="B7" s="159" t="s">
         <v>439</v>
       </c>
@@ -11306,7 +11306,7 @@
       <c r="AH7" s="108"/>
     </row>
     <row r="8" spans="1:47" s="105" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A8" s="201"/>
+      <c r="A8" s="219"/>
       <c r="B8" s="160" t="s">
         <v>432</v>
       </c>
@@ -11392,7 +11392,7 @@
       <c r="AH8" s="108"/>
     </row>
     <row r="9" spans="1:47" s="105" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A9" s="199"/>
+      <c r="A9" s="217"/>
       <c r="B9" s="161" t="s">
         <v>21</v>
       </c>
@@ -11468,7 +11468,7 @@
       <c r="AH9" s="108"/>
     </row>
     <row r="10" spans="1:47" s="107" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A10" s="198" t="s">
+      <c r="A10" s="216" t="s">
         <v>454</v>
       </c>
       <c r="B10" s="158" t="s">
@@ -11571,7 +11571,7 @@
       <c r="AU10" s="105"/>
     </row>
     <row r="11" spans="1:47" s="107" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A11" s="199"/>
+      <c r="A11" s="217"/>
       <c r="B11" s="158" t="s">
         <v>453</v>
       </c>
@@ -11779,7 +11779,7 @@
       <c r="AU12" s="105"/>
     </row>
     <row r="13" spans="1:47" s="107" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A13" s="202" t="s">
+      <c r="A13" s="220" t="s">
         <v>374</v>
       </c>
       <c r="B13" s="162" t="s">
@@ -11886,7 +11886,7 @@
       <c r="AU13" s="105"/>
     </row>
     <row r="14" spans="1:47" s="107" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A14" s="203"/>
+      <c r="A14" s="221"/>
       <c r="B14" s="162" t="s">
         <v>358</v>
       </c>
@@ -11989,7 +11989,7 @@
       <c r="AU14" s="105"/>
     </row>
     <row r="15" spans="1:47" ht="14.5" customHeight="1">
-      <c r="A15" s="204" t="s">
+      <c r="A15" s="222" t="s">
         <v>470</v>
       </c>
       <c r="B15" s="161" t="s">
@@ -12087,7 +12087,7 @@
       <c r="AH15" s="108"/>
     </row>
     <row r="16" spans="1:47" s="104" customFormat="1" ht="14.5" customHeight="1">
-      <c r="A16" s="205"/>
+      <c r="A16" s="223"/>
       <c r="B16" s="163" t="s">
         <v>499</v>
       </c>
@@ -12196,7 +12196,7 @@
       <c r="AU16" s="1"/>
     </row>
     <row r="17" spans="1:47" ht="14.5" customHeight="1">
-      <c r="A17" s="205"/>
+      <c r="A17" s="223"/>
       <c r="B17" s="163" t="s">
         <v>498</v>
       </c>
@@ -12292,7 +12292,7 @@
       <c r="AH17" s="108"/>
     </row>
     <row r="18" spans="1:47" ht="14.5" customHeight="1">
-      <c r="A18" s="205"/>
+      <c r="A18" s="223"/>
       <c r="B18" s="164" t="s">
         <v>497</v>
       </c>
@@ -12388,7 +12388,7 @@
       <c r="AH18" s="108"/>
     </row>
     <row r="19" spans="1:47" ht="15" customHeight="1" thickBot="1">
-      <c r="A19" s="206"/>
+      <c r="A19" s="224"/>
       <c r="B19" s="159" t="s">
         <v>302</v>
       </c>
@@ -12480,7 +12480,7 @@
       <c r="AH19" s="108"/>
     </row>
     <row r="20" spans="1:47" s="105" customFormat="1" ht="14.5" customHeight="1">
-      <c r="A20" s="198" t="s">
+      <c r="A20" s="216" t="s">
         <v>424</v>
       </c>
       <c r="B20" s="161" t="s">
@@ -12513,7 +12513,7 @@
       <c r="K20" s="111">
         <v>2</v>
       </c>
-      <c r="L20" s="207" t="s">
+      <c r="L20" s="211" t="s">
         <v>451</v>
       </c>
       <c r="M20" s="111" t="s">
@@ -12578,7 +12578,7 @@
       <c r="AH20" s="108"/>
     </row>
     <row r="21" spans="1:47" s="105" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A21" s="201"/>
+      <c r="A21" s="219"/>
       <c r="B21" s="159" t="s">
         <v>495</v>
       </c>
@@ -12609,7 +12609,7 @@
       <c r="K21" s="111">
         <v>2</v>
       </c>
-      <c r="L21" s="208"/>
+      <c r="L21" s="212"/>
       <c r="M21" s="111" t="s">
         <v>450</v>
       </c>
@@ -12672,7 +12672,7 @@
       <c r="AH21" s="108"/>
     </row>
     <row r="22" spans="1:47" s="107" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A22" s="199"/>
+      <c r="A22" s="217"/>
       <c r="B22" s="162" t="s">
         <v>494</v>
       </c>
@@ -13454,7 +13454,7 @@
         <v>443</v>
       </c>
       <c r="AE30" s="111" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="AF30" s="111"/>
       <c r="AG30" s="111"/>
@@ -13904,7 +13904,7 @@
       <c r="AU38" s="1"/>
     </row>
     <row r="39" spans="1:47" s="103" customFormat="1" ht="17" thickTop="1">
-      <c r="A39" s="198" t="s">
+      <c r="A39" s="216" t="s">
         <v>16</v>
       </c>
       <c r="B39" s="165" t="s">
@@ -13999,7 +13999,7 @@
       <c r="AU39" s="1"/>
     </row>
     <row r="40" spans="1:47" s="103" customFormat="1" ht="17" thickBot="1">
-      <c r="A40" s="199"/>
+      <c r="A40" s="217"/>
       <c r="B40" s="166" t="s">
         <v>340</v>
       </c>
@@ -14092,7 +14092,7 @@
       <c r="AU40" s="1"/>
     </row>
     <row r="41" spans="1:47" s="103" customFormat="1" ht="17" thickBot="1">
-      <c r="A41" s="200" t="s">
+      <c r="A41" s="218" t="s">
         <v>28</v>
       </c>
       <c r="B41" s="161" t="s">
@@ -14185,7 +14185,7 @@
       <c r="AU41" s="1"/>
     </row>
     <row r="42" spans="1:47" s="103" customFormat="1" ht="17" thickBot="1">
-      <c r="A42" s="200"/>
+      <c r="A42" s="218"/>
       <c r="B42" s="159" t="s">
         <v>493</v>
       </c>
@@ -14987,18 +14987,13 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="AF2:AH2"/>
-    <mergeCell ref="AF3:AF4"/>
-    <mergeCell ref="AG3:AG4"/>
-    <mergeCell ref="AH3:AH4"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="S2:X2"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A5:A9"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A19"/>
     <mergeCell ref="L20:L21"/>
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="Y2:AD2"/>
@@ -15015,13 +15010,18 @@
     <mergeCell ref="U3:U4"/>
     <mergeCell ref="V3:V4"/>
     <mergeCell ref="W3:W4"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A5:A9"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="AF2:AH2"/>
+    <mergeCell ref="AF3:AF4"/>
+    <mergeCell ref="AG3:AG4"/>
+    <mergeCell ref="AH3:AH4"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="S2:X2"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="I3:J3"/>
   </mergeCells>
   <phoneticPr fontId="21" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>